<commit_message>
trade off result sumsel & Sulsel + BAU data for jabar
</commit_message>
<xml_diff>
--- a/_DB/data/SumSel/Building LRC Rate based on Jabar's.xlsx
+++ b/_DB/data/SumSel/Building LRC Rate based on Jabar's.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icrafguest01\tin\pprk_apps_tinbaru\aksara_rancang\_DB\data\SumSel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB59001-38E2-4EB1-B283-4A8170B0F85D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F30C20-AA0C-4293-812A-DBD9CD36963C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3E4B5BF1-7876-4422-A9D8-101145E56EBA}"/>
   </bookViews>
@@ -822,34 +822,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE787D96-9BE1-41B3-ACF7-C69305D0C41F}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C62"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="55.140625" customWidth="1"/>
+    <col min="3" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -857,24 +857,27 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>F2</f>
+        <f>G2</f>
         <v>0.96153846200000004</v>
       </c>
       <c r="D2">
+        <v>0.96</v>
+      </c>
+      <c r="E2">
         <f>C2*1.003</f>
         <v>0.96442307738599997</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>63</v>
-      </c>
-      <c r="F2">
-        <v>0.96153846200000004</v>
       </c>
       <c r="G2">
         <v>0.96153846200000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0.96153846200000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -882,23 +885,26 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f>F3</f>
+        <f>G3</f>
         <v>1.0204081629999999</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1.0204081629999999</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -906,24 +912,27 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <f>F2</f>
+        <f>G2</f>
         <v>0.96153846200000004</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D3:D61" si="0">C4*1.003</f>
+        <v>0.96</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E61" si="0">C4*1.003</f>
         <v>0.96442307738599997</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="F4">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G4">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -931,24 +940,27 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <f>F2</f>
+        <f>G2</f>
         <v>0.96153846200000004</v>
       </c>
       <c r="D5">
+        <v>0.96</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>0.96442307738599997</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5">
-        <v>0.92592592600000001</v>
       </c>
       <c r="G5">
         <v>0.92592592600000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0.92592592600000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -956,23 +968,26 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <f>F3</f>
+        <f>G3</f>
         <v>1.0204081629999999</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>66</v>
-      </c>
-      <c r="F6">
-        <v>0.92592592600000001</v>
       </c>
       <c r="G6">
         <v>0.92592592600000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0.92592592600000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -980,24 +995,27 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <f>F4</f>
+        <f>G4</f>
         <v>0.90090090099999998</v>
       </c>
       <c r="D7">
+        <v>0.96</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>67</v>
-      </c>
-      <c r="F7">
-        <v>0.94339622599999995</v>
       </c>
       <c r="G7">
         <v>0.94339622599999995</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0.94339622599999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1009,20 +1027,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D8">
+        <v>0.96</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>17</v>
-      </c>
-      <c r="F8">
-        <v>0.89285714299999996</v>
       </c>
       <c r="G8">
         <v>0.89285714299999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0.89285714299999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1034,20 +1055,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D9">
+        <v>0.96</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>68</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1.0416666670000001</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1059,20 +1083,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D10">
+        <v>0.96</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>69</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1.0416666670000001</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1084,20 +1111,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D11">
+        <v>0.96</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>70</v>
-      </c>
-      <c r="F11">
-        <v>0.81967213100000003</v>
       </c>
       <c r="G11">
         <v>0.81967213100000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>0.81967213100000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1109,20 +1139,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D12">
+        <v>0.96</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>71</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1.111111111</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1.2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1134,20 +1167,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D13">
+        <v>0.96</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>72</v>
-      </c>
-      <c r="F13">
-        <v>0.79365079400000005</v>
       </c>
       <c r="G13">
         <v>0.79365079400000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>0.79365079400000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1159,20 +1195,23 @@
         <v>0.90090090099999998</v>
       </c>
       <c r="D14">
+        <v>0.96</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>73</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1.923076923</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1180,24 +1219,27 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <f>$F$6</f>
+        <f>$G$6</f>
         <v>0.92592592600000001</v>
       </c>
       <c r="D15">
+        <v>0.96</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>0.92870370377799993</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>74</v>
-      </c>
-      <c r="F15">
-        <v>0.71942446000000004</v>
       </c>
       <c r="G15">
         <v>0.71942446000000004</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>0.71942446000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1205,24 +1247,27 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C17" si="2">$F$6</f>
+        <f t="shared" ref="C16:C17" si="2">$G$6</f>
         <v>0.92592592600000001</v>
       </c>
       <c r="D16">
+        <v>0.96</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>0.92870370377799993</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>75</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1.0204081629999999</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1234,20 +1279,23 @@
         <v>0.92592592600000001</v>
       </c>
       <c r="D17">
+        <v>0.96</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>0.92870370377799993</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>76</v>
-      </c>
-      <c r="F17">
-        <v>0.81967213100000003</v>
       </c>
       <c r="G17">
         <v>0.81967213100000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>0.81967213100000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1255,24 +1303,27 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <f>F7</f>
+        <f>G7</f>
         <v>0.94339622599999995</v>
       </c>
       <c r="D18">
+        <v>0.96</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>0.94622641467799984</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>77</v>
-      </c>
-      <c r="F18">
-        <v>0.78740157499999996</v>
       </c>
       <c r="G18">
         <v>0.78740157499999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0.78740157499999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1280,24 +1331,27 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <f>F8</f>
+        <f>G8</f>
         <v>0.89285714299999996</v>
       </c>
       <c r="D19">
+        <v>0.96</v>
+      </c>
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>0.89553571442899982</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>78</v>
-      </c>
-      <c r="F19">
-        <v>0.909090909</v>
       </c>
       <c r="G19">
         <v>0.909090909</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0.909090909</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1305,24 +1359,27 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <f>F11</f>
+        <f>G11</f>
         <v>0.81967213100000003</v>
       </c>
       <c r="D20">
+        <v>0.88</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>0.82213114739299997</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>79</v>
-      </c>
-      <c r="F20">
-        <v>0.81967213100000003</v>
       </c>
       <c r="G20">
         <v>0.81967213100000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0.81967213100000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1330,24 +1387,27 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <f>F11</f>
+        <f>G11</f>
         <v>0.81967213100000003</v>
       </c>
       <c r="D21">
+        <v>0.88</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="0"/>
         <v>0.82213114739299997</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>80</v>
-      </c>
-      <c r="F21">
-        <v>0.88495575199999998</v>
       </c>
       <c r="G21">
         <v>0.88495575199999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0.88495575199999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1355,24 +1415,27 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <f>F9</f>
+        <f>G9</f>
         <v>1.0416666670000001</v>
       </c>
       <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>1.044791667001</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>81</v>
-      </c>
-      <c r="F22">
-        <v>0.625</v>
       </c>
       <c r="G22">
         <v>0.625</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1380,24 +1443,27 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <f>F11</f>
+        <f>G11</f>
         <v>0.81967213100000003</v>
       </c>
       <c r="D23">
+        <v>0.88</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>0.82213114739299997</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>82</v>
-      </c>
-      <c r="F23">
-        <v>0.54347826099999996</v>
       </c>
       <c r="G23">
         <v>0.54347826099999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0.54347826099999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1405,23 +1471,26 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <f>F13</f>
+        <f>G13</f>
         <v>0.79365079400000005</v>
       </c>
       <c r="D24">
+        <v>0.8</v>
+      </c>
+      <c r="E24">
         <v>0.81</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>83</v>
-      </c>
-      <c r="F24">
-        <v>0.99009901</v>
       </c>
       <c r="G24">
         <v>0.99009901</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0.99009901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1429,23 +1498,26 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <f t="shared" ref="C25:C27" si="3">$F$13</f>
+        <f t="shared" ref="C25:C27" si="3">$G$13</f>
         <v>0.79365079400000005</v>
       </c>
       <c r="D25">
+        <v>0.8</v>
+      </c>
+      <c r="E25">
         <v>0.81</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>84</v>
-      </c>
-      <c r="F25">
-        <v>0.92592592600000001</v>
       </c>
       <c r="G25">
         <v>0.92592592600000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>0.92592592600000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1457,19 +1529,22 @@
         <v>0.79365079400000005</v>
       </c>
       <c r="D26">
+        <v>0.8</v>
+      </c>
+      <c r="E26">
         <v>0.81</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>85</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>1.075268817</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1481,19 +1556,22 @@
         <v>0.79365079400000005</v>
       </c>
       <c r="D27">
+        <v>0.8</v>
+      </c>
+      <c r="E27">
         <v>0.81</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>86</v>
       </c>
-      <c r="F27">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G27">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1501,23 +1579,26 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <f>$F$13</f>
+        <f>$G$13</f>
         <v>0.79365079400000005</v>
       </c>
       <c r="D28">
+        <v>0.8</v>
+      </c>
+      <c r="E28">
         <v>0.81</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>87</v>
-      </c>
-      <c r="F28">
-        <v>0.91743119299999998</v>
       </c>
       <c r="G28">
         <v>0.91743119299999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0.91743119299999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1525,23 +1606,26 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <f>F13</f>
+        <f>G13</f>
         <v>0.79365079400000005</v>
       </c>
       <c r="D29">
+        <v>0.8</v>
+      </c>
+      <c r="E29">
         <v>0.81</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>88</v>
-      </c>
-      <c r="F29">
-        <v>0.78125</v>
       </c>
       <c r="G29">
         <v>0.78125</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1549,23 +1633,26 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <f>F13</f>
+        <f>G13</f>
         <v>0.79365079400000005</v>
       </c>
       <c r="D30">
+        <v>0.8</v>
+      </c>
+      <c r="E30">
         <v>0.81</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>89</v>
-      </c>
-      <c r="F30">
-        <v>0.909090909</v>
       </c>
       <c r="G30">
         <v>0.909090909</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0.909090909</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1578,17 +1665,20 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
         <v>90</v>
-      </c>
-      <c r="F31">
-        <v>0.746268657</v>
       </c>
       <c r="G31">
         <v>0.746268657</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>0.746268657</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1596,24 +1686,27 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <f>AVERAGE(F15:F16)</f>
+        <f>AVERAGE(G15:G16)</f>
         <v>0.86991631149999993</v>
       </c>
       <c r="D32">
+        <v>0.86</v>
+      </c>
+      <c r="E32">
         <f t="shared" si="0"/>
         <v>0.87252606043449987</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>91</v>
       </c>
-      <c r="F32">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G32">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1621,24 +1714,27 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <f>F17</f>
+        <f>G17</f>
         <v>0.81967213100000003</v>
       </c>
       <c r="D33">
+        <v>0.8</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="0"/>
         <v>0.82213114739299997</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>92</v>
       </c>
-      <c r="F33">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G33">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1646,24 +1742,27 @@
         <v>32</v>
       </c>
       <c r="C34">
-        <f>F18</f>
+        <f>G18</f>
         <v>0.78740157499999996</v>
       </c>
       <c r="D34">
+        <v>0.8</v>
+      </c>
+      <c r="E34">
         <f t="shared" si="0"/>
         <v>0.78976377972499989</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>93</v>
-      </c>
-      <c r="F34">
-        <v>0.84033613399999996</v>
       </c>
       <c r="G34">
         <v>0.84033613399999996</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>0.84033613399999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1671,24 +1770,27 @@
         <v>33</v>
       </c>
       <c r="C35">
-        <f>F19</f>
+        <f>G19</f>
         <v>0.909090909</v>
       </c>
       <c r="D35">
+        <v>0.9</v>
+      </c>
+      <c r="E35">
         <f t="shared" si="0"/>
         <v>0.91181818172699991</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>94</v>
       </c>
-      <c r="F35">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G35">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1696,24 +1798,27 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <f>F19</f>
+        <f>G19</f>
         <v>0.909090909</v>
       </c>
       <c r="D36">
+        <v>0.9</v>
+      </c>
+      <c r="E36">
         <f t="shared" si="0"/>
         <v>0.91181818172699991</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>95</v>
-      </c>
-      <c r="F36">
-        <v>0.98039215700000004</v>
       </c>
       <c r="G36">
         <v>0.98039215700000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>0.98039215700000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1725,20 +1830,23 @@
         <v>0.9</v>
       </c>
       <c r="D37">
+        <v>0.9</v>
+      </c>
+      <c r="E37">
         <f t="shared" si="0"/>
         <v>0.90269999999999995</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>96</v>
-      </c>
-      <c r="F37">
-        <v>0.98039215700000004</v>
       </c>
       <c r="G37">
         <v>0.98039215700000004</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>0.98039215700000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1746,24 +1854,27 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <f>F20</f>
+        <f>G20</f>
         <v>0.81967213100000003</v>
       </c>
       <c r="D38">
+        <v>0.8</v>
+      </c>
+      <c r="E38">
         <f t="shared" si="0"/>
         <v>0.82213114739299997</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>97</v>
-      </c>
-      <c r="F38">
-        <v>0.83333333300000001</v>
       </c>
       <c r="G38">
         <v>0.83333333300000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>0.83333333300000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1771,24 +1882,27 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <f>F21</f>
+        <f>G21</f>
         <v>0.88495575199999998</v>
       </c>
       <c r="D39">
+        <v>0.88</v>
+      </c>
+      <c r="E39">
         <f t="shared" si="0"/>
         <v>0.88761061925599993</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>98</v>
-      </c>
-      <c r="F39">
-        <v>0.82644628099999995</v>
       </c>
       <c r="G39">
         <v>0.82644628099999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>0.82644628099999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1796,24 +1910,27 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <f>F21</f>
+        <f>G21</f>
         <v>0.88495575199999998</v>
       </c>
       <c r="D40">
+        <v>0.88</v>
+      </c>
+      <c r="E40">
         <f t="shared" si="0"/>
         <v>0.88761061925599993</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>99</v>
       </c>
-      <c r="F40">
-        <v>0.90090090099999998</v>
-      </c>
       <c r="G40">
         <v>0.90090090099999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0.90090090099999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1821,24 +1938,27 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <f>F22</f>
+        <f>G22</f>
         <v>0.625</v>
       </c>
       <c r="D41">
+        <v>0.88</v>
+      </c>
+      <c r="E41">
         <f t="shared" si="0"/>
         <v>0.62687499999999996</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>100</v>
-      </c>
-      <c r="F41">
-        <v>0.84745762700000005</v>
       </c>
       <c r="G41">
         <v>0.84745762700000005</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>0.84745762700000005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1846,24 +1966,27 @@
         <v>40</v>
       </c>
       <c r="C42">
-        <f>F21</f>
+        <f>G21</f>
         <v>0.88495575199999998</v>
       </c>
       <c r="D42">
+        <v>0.88</v>
+      </c>
+      <c r="E42">
         <f t="shared" si="0"/>
         <v>0.88761061925599993</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>101</v>
-      </c>
-      <c r="F42">
-        <v>0.68965517200000004</v>
       </c>
       <c r="G42">
         <v>0.68965517200000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0.68965517200000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1871,24 +1994,27 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <f>F23</f>
+        <f>G23</f>
         <v>0.54347826099999996</v>
       </c>
       <c r="D43">
+        <v>0.88</v>
+      </c>
+      <c r="E43">
         <f t="shared" si="0"/>
         <v>0.54510869578299992</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>102</v>
-      </c>
-      <c r="F43">
-        <v>0.80645161300000001</v>
       </c>
       <c r="G43">
         <v>0.80645161300000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0.80645161300000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1896,24 +2022,27 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <f>F24</f>
+        <f>G24</f>
         <v>0.99009901</v>
       </c>
       <c r="D44">
+        <v>0.88</v>
+      </c>
+      <c r="E44">
         <f t="shared" si="0"/>
         <v>0.99306930702999985</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>103</v>
-      </c>
-      <c r="F44">
-        <v>0.80645161300000001</v>
       </c>
       <c r="G44">
         <v>0.80645161300000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0.80645161300000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1921,24 +2050,27 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <f>F24</f>
+        <f>G24</f>
         <v>0.99009901</v>
       </c>
       <c r="D45">
+        <v>0.88</v>
+      </c>
+      <c r="E45">
         <f t="shared" si="0"/>
         <v>0.99306930702999985</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>104</v>
-      </c>
-      <c r="F45">
-        <v>0.80645161300000001</v>
       </c>
       <c r="G45">
         <v>0.80645161300000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>0.80645161300000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1946,24 +2078,27 @@
         <v>44</v>
       </c>
       <c r="C46">
-        <f>F27</f>
+        <f>G27</f>
         <v>0.90090090099999998</v>
       </c>
       <c r="D46">
+        <v>0.88</v>
+      </c>
+      <c r="E46">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>105</v>
-      </c>
-      <c r="F46">
-        <v>0.80645161300000001</v>
       </c>
       <c r="G46">
         <v>0.80645161300000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>0.80645161300000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1971,24 +2106,27 @@
         <v>45</v>
       </c>
       <c r="C47">
-        <f>AVERAGE(F29:F30)</f>
+        <f>AVERAGE(G29:G30)</f>
         <v>0.84517045450000006</v>
       </c>
       <c r="D47">
+        <v>0.88</v>
+      </c>
+      <c r="E47">
         <f t="shared" si="0"/>
         <v>0.8477059658635</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>106</v>
-      </c>
-      <c r="F47">
-        <v>0.84745762700000005</v>
       </c>
       <c r="G47">
         <v>0.84745762700000005</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>0.84745762700000005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1996,24 +2134,27 @@
         <v>46</v>
       </c>
       <c r="C48">
-        <f>F31</f>
+        <f>G31</f>
         <v>0.746268657</v>
       </c>
       <c r="D48">
+        <v>0.88</v>
+      </c>
+      <c r="E48">
         <f t="shared" si="0"/>
         <v>0.7485074629709999</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>107</v>
-      </c>
-      <c r="F48">
-        <v>0.82644628099999995</v>
       </c>
       <c r="G48">
         <v>0.82644628099999995</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>0.82644628099999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2021,24 +2162,27 @@
         <v>47</v>
       </c>
       <c r="C49">
-        <f>F32</f>
+        <f>G32</f>
         <v>0.90090090099999998</v>
       </c>
       <c r="D49">
+        <v>0.88</v>
+      </c>
+      <c r="E49">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>108</v>
-      </c>
-      <c r="F49">
-        <v>0.98039215700000004</v>
       </c>
       <c r="G49">
         <v>0.98039215700000004</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>0.98039215700000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2046,24 +2190,27 @@
         <v>48</v>
       </c>
       <c r="C50">
-        <f>AVERAGE(F40:F41)</f>
+        <f>AVERAGE(G40:G41)</f>
         <v>0.87417926400000001</v>
       </c>
       <c r="D50">
+        <v>0.88</v>
+      </c>
+      <c r="E50">
         <f t="shared" si="0"/>
         <v>0.87680180179199996</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>109</v>
-      </c>
-      <c r="F50">
-        <v>0.8</v>
       </c>
       <c r="G50">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2071,24 +2218,27 @@
         <v>49</v>
       </c>
       <c r="C51">
-        <f>F34</f>
+        <f>G34</f>
         <v>0.84033613399999996</v>
       </c>
       <c r="D51">
+        <v>0.88</v>
+      </c>
+      <c r="E51">
         <f t="shared" si="0"/>
         <v>0.84285714240199983</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>110</v>
-      </c>
-      <c r="F51">
-        <v>0.71942446000000004</v>
       </c>
       <c r="G51">
         <v>0.71942446000000004</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>0.71942446000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2096,24 +2246,27 @@
         <v>50</v>
       </c>
       <c r="C52">
-        <f>F35</f>
+        <f>G35</f>
         <v>0.90090090099999998</v>
       </c>
       <c r="D52">
+        <v>0.88</v>
+      </c>
+      <c r="E52">
         <f t="shared" si="0"/>
         <v>0.90360360370299986</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>111</v>
-      </c>
-      <c r="F52">
-        <v>0.94339622599999995</v>
       </c>
       <c r="G52">
         <v>0.94339622599999995</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>0.94339622599999995</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2121,24 +2274,27 @@
         <v>51</v>
       </c>
       <c r="C53">
-        <f>F36</f>
+        <f>G36</f>
         <v>0.98039215700000004</v>
       </c>
       <c r="D53">
+        <v>0.88</v>
+      </c>
+      <c r="E53">
         <f t="shared" si="0"/>
         <v>0.98333333347099994</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>112</v>
-      </c>
-      <c r="F53">
-        <v>0.96153846200000004</v>
       </c>
       <c r="G53">
         <v>0.96153846200000004</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>0.96153846200000004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2146,21 +2302,24 @@
         <v>52</v>
       </c>
       <c r="C54">
-        <f>F38</f>
+        <f>G38</f>
         <v>0.83333333300000001</v>
       </c>
       <c r="D54">
+        <v>0.88</v>
+      </c>
+      <c r="E54">
         <f t="shared" si="0"/>
         <v>0.83583333299899987</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2168,15 +2327,18 @@
         <v>53</v>
       </c>
       <c r="C55">
-        <f>F42</f>
+        <f>G42</f>
         <v>0.68965517200000004</v>
       </c>
       <c r="D55">
+        <v>0.88</v>
+      </c>
+      <c r="E55">
         <f t="shared" si="0"/>
         <v>0.69172413751599993</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2184,15 +2346,18 @@
         <v>54</v>
       </c>
       <c r="C56">
-        <f>F43</f>
+        <f>G43</f>
         <v>0.80645161300000001</v>
       </c>
       <c r="D56">
+        <v>0.88</v>
+      </c>
+      <c r="E56">
         <f t="shared" si="0"/>
         <v>0.80887096783899992</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2200,15 +2365,18 @@
         <v>55</v>
       </c>
       <c r="C57">
-        <f>F48</f>
+        <f>G48</f>
         <v>0.82644628099999995</v>
       </c>
       <c r="D57">
+        <v>0.88</v>
+      </c>
+      <c r="E57">
         <f t="shared" si="0"/>
         <v>0.82892561984299984</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2216,15 +2384,18 @@
         <v>56</v>
       </c>
       <c r="C58">
-        <f>F49</f>
+        <f>G49</f>
         <v>0.98039215700000004</v>
       </c>
       <c r="D58">
+        <v>0.88</v>
+      </c>
+      <c r="E58">
         <f t="shared" si="0"/>
         <v>0.98333333347099994</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2232,14 +2403,17 @@
         <v>57</v>
       </c>
       <c r="C59">
-        <f>F51</f>
+        <f>G51</f>
         <v>0.71942446000000004</v>
       </c>
       <c r="D59">
+        <v>0.88</v>
+      </c>
+      <c r="E59">
         <v>0.8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2247,15 +2421,18 @@
         <v>58</v>
       </c>
       <c r="C60">
-        <f>F52</f>
+        <f>G52</f>
         <v>0.94339622599999995</v>
       </c>
       <c r="D60">
+        <v>0.88</v>
+      </c>
+      <c r="E60">
         <f t="shared" si="0"/>
         <v>0.94622641467799984</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2263,15 +2440,18 @@
         <v>59</v>
       </c>
       <c r="C61">
-        <f>F54</f>
+        <f>G54</f>
         <v>0</v>
       </c>
       <c r="D61">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>145</v>
       </c>
@@ -2279,6 +2459,9 @@
         <v>0</v>
       </c>
       <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
         <v>0</v>
       </c>
     </row>

</xml_diff>